<commit_message>
Removed the need for LocationID in Price data
</commit_message>
<xml_diff>
--- a/Templates/PriceTemplate.xlsx
+++ b/Templates/PriceTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/690b8719eb6b5234/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\source\repos\HCarlb\FinancePriceCalculator\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{44A95B37-8F06-4394-BF3F-9D5B19C0A435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7C1FC605-733D-4D7C-A3F5-10D588940687}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A2B4F0-742A-462A-9B9E-FD96ED818E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{971169AE-1140-4A36-B9DA-0B1E2CF5C788}"/>
   </bookViews>
@@ -33,18 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
-  <si>
-    <t>LocationID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ProductID</t>
   </si>
   <si>
     <t>MaterialPrice</t>
-  </si>
-  <si>
-    <t>ABC</t>
   </si>
   <si>
     <t>ABC123</t>
@@ -408,71 +402,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B58D631-15DA-4379-93F6-A1864836A515}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2">
+        <v>10.199999999999999</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
         <v>654</v>
       </c>
     </row>

</xml_diff>